<commit_message>
Better OOP Header and Row
</commit_message>
<xml_diff>
--- a/examples/example.xlsx
+++ b/examples/example.xlsx
@@ -184,24 +184,24 @@
         </is>
       </c>
     </row>
-    <row collapsed="" customFormat="false" customHeight="" hidden="" ht="12.1" outlineLevel="0" r="2">
+    <row collapsed="" customFormat="false" customHeight="1" hidden="" ht="30" outlineLevel="0" r="2">
       <c r="A2" s="4" t="inlineStr">
         <is>
           <t>Value1</t>
         </is>
       </c>
       <c r="B2" s="5" t="n">
-        <v>43799.668784722</v>
+        <v>43799.689259259</v>
       </c>
     </row>
-    <row collapsed="" customFormat="false" customHeight="" hidden="" ht="12.1" outlineLevel="0" r="3">
+    <row collapsed="" customFormat="false" customHeight="1" hidden="" ht="30" outlineLevel="0" r="3">
       <c r="A3" s="4" t="inlineStr">
         <is>
           <t>Value2</t>
         </is>
       </c>
       <c r="B3" s="5" t="n">
-        <v>43799.668784722</v>
+        <v>43799.689259259</v>
       </c>
     </row>
   </sheetData>

</xml_diff>